<commit_message>
trying to find pattern for rbar and gamma estimates
</commit_message>
<xml_diff>
--- a/results/gamma_estimates.xlsx
+++ b/results/gamma_estimates.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="10335"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="10335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="37">
   <si>
     <t>All</t>
   </si>
@@ -100,6 +102,42 @@
   <si>
     <t>4CO shape</t>
   </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>2CO</t>
+  </si>
+  <si>
+    <t>3CO</t>
+  </si>
+  <si>
+    <t>4CO</t>
+  </si>
+  <si>
+    <t>type.IFD</t>
+  </si>
+  <si>
+    <t>strain</t>
+  </si>
+  <si>
+    <t>All.Strain</t>
+  </si>
+  <si>
+    <t>all.Biv</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>All.Strains</t>
+  </si>
 </sst>
 </file>
 
@@ -143,7 +181,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -255,11 +293,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -290,6 +352,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +658,8 @@
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.28515625" customWidth="1"/>
     <col min="13" max="13" width="4.42578125" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.140625" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" customWidth="1"/>
     <col min="21" max="21" width="4.7109375" customWidth="1"/>
     <col min="22" max="22" width="9.5703125" customWidth="1"/>
   </cols>
@@ -2147,4 +2217,3945 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="11">
+        <v>3.8</v>
+      </c>
+      <c r="D2" s="11">
+        <v>13.9</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1697</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>3.1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>15.5</v>
+      </c>
+      <c r="E3" s="9">
+        <v>252</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="D4" s="9">
+        <v>11.3</v>
+      </c>
+      <c r="E4" s="9">
+        <v>310</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>5.2</v>
+      </c>
+      <c r="D5" s="9">
+        <v>10.9</v>
+      </c>
+      <c r="E5" s="9">
+        <v>284</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="11">
+        <v>3.8</v>
+      </c>
+      <c r="D6" s="11">
+        <v>13.8</v>
+      </c>
+      <c r="E6" s="9">
+        <v>357</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="11">
+        <v>4.3</v>
+      </c>
+      <c r="D7" s="9">
+        <v>14.5</v>
+      </c>
+      <c r="E7" s="9">
+        <v>138</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9">
+        <v>16</v>
+      </c>
+      <c r="E8" s="9">
+        <v>153</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="9">
+        <v>3.9</v>
+      </c>
+      <c r="D9" s="9">
+        <v>14.7</v>
+      </c>
+      <c r="E9" s="9">
+        <v>203</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="11">
+        <v>4.8</v>
+      </c>
+      <c r="D10" s="11">
+        <v>12</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1355</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <v>3.6</v>
+      </c>
+      <c r="D11" s="9">
+        <v>14.7</v>
+      </c>
+      <c r="E11" s="9">
+        <v>186</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="9">
+        <v>5.6</v>
+      </c>
+      <c r="D12" s="9">
+        <v>9.6</v>
+      </c>
+      <c r="E12" s="9">
+        <v>245</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="9">
+        <v>7.1</v>
+      </c>
+      <c r="D13" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="E13" s="9">
+        <v>240</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D14" s="9">
+        <v>11.6</v>
+      </c>
+      <c r="E14" s="9">
+        <v>285</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="D15" s="9">
+        <v>14.1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>128</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="9">
+        <v>4</v>
+      </c>
+      <c r="D16" s="9">
+        <v>14</v>
+      </c>
+      <c r="E16" s="9">
+        <v>113</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9">
+        <v>4.7</v>
+      </c>
+      <c r="D17" s="9">
+        <v>13</v>
+      </c>
+      <c r="E17" s="9">
+        <v>158</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="11">
+        <v>2.8</v>
+      </c>
+      <c r="D18" s="11">
+        <v>13.6</v>
+      </c>
+      <c r="E18" s="11">
+        <v>318</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9">
+        <v>3</v>
+      </c>
+      <c r="D19" s="9">
+        <v>11</v>
+      </c>
+      <c r="E19" s="9">
+        <v>60</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="9">
+        <v>3.1</v>
+      </c>
+      <c r="D20" s="9">
+        <v>13.4</v>
+      </c>
+      <c r="E20" s="9">
+        <v>56</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="D21" s="9">
+        <v>12.6</v>
+      </c>
+      <c r="E21" s="9">
+        <v>38</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="9">
+        <v>3</v>
+      </c>
+      <c r="D22" s="9">
+        <v>12</v>
+      </c>
+      <c r="E22" s="9">
+        <v>72</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="D23" s="9">
+        <v>15.8</v>
+      </c>
+      <c r="E23" s="9">
+        <v>10</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D24" s="9">
+        <v>15.7</v>
+      </c>
+      <c r="E24" s="9">
+        <v>40</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="9">
+        <v>3.1</v>
+      </c>
+      <c r="D25" s="9">
+        <v>14.7</v>
+      </c>
+      <c r="E25" s="9">
+        <v>42</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="11">
+        <v>3.7</v>
+      </c>
+      <c r="D26" s="11">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E26" s="11">
+        <v>24</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D27" s="19">
+        <v>5.9</v>
+      </c>
+      <c r="E27" s="19">
+        <v>6</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="11">
+        <v>3.4</v>
+      </c>
+      <c r="D28" s="11">
+        <v>9.6</v>
+      </c>
+      <c r="E28" s="19">
+        <v>9</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="11">
+        <v>3.4</v>
+      </c>
+      <c r="D29" s="19">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E29" s="19">
+        <v>6</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="11">
+        <v>4.2</v>
+      </c>
+      <c r="D30" s="19">
+        <v>5.6</v>
+      </c>
+      <c r="E30" s="19">
+        <v>3</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="11">
+        <v>4.8380000000000001</v>
+      </c>
+      <c r="D31" s="11">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="E31" s="9">
+        <v>1697</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="11">
+        <v>3.73</v>
+      </c>
+      <c r="D32" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E32" s="9">
+        <v>252</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="11">
+        <v>5.4390000000000001</v>
+      </c>
+      <c r="D33" s="11">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="E33" s="9">
+        <v>310</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="11">
+        <v>6.319</v>
+      </c>
+      <c r="D34" s="11">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="E34" s="9">
+        <v>284</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="11">
+        <v>4.8440000000000003</v>
+      </c>
+      <c r="D35" s="11">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="E35" s="9">
+        <v>357</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="11">
+        <v>6.3979999999999997</v>
+      </c>
+      <c r="D36" s="11">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="E36" s="9">
+        <v>138</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="11">
+        <v>3.87</v>
+      </c>
+      <c r="D37" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E37" s="9">
+        <v>153</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="11">
+        <v>4.7539999999999996</v>
+      </c>
+      <c r="D38" s="11">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="E38" s="9">
+        <v>203</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="11">
+        <v>6.92</v>
+      </c>
+      <c r="D39" s="11">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="E39" s="11">
+        <v>1355</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D40" s="11">
+        <v>0.09</v>
+      </c>
+      <c r="E40" s="11">
+        <v>186</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="11">
+        <v>7.4130000000000003</v>
+      </c>
+      <c r="D41" s="11">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E41" s="11">
+        <v>245</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="18">
+        <v>9.83</v>
+      </c>
+      <c r="D42" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="E42" s="11">
+        <v>240</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="11">
+        <v>6.7460000000000004</v>
+      </c>
+      <c r="D43" s="11">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="E43" s="11">
+        <v>285</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="11">
+        <v>7.4130000000000003</v>
+      </c>
+      <c r="D44" s="11">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="E44" s="11">
+        <v>128</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="11">
+        <v>5.8090000000000002</v>
+      </c>
+      <c r="D45" s="11">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="E45" s="11">
+        <v>113</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="11">
+        <v>7.2320000000000002</v>
+      </c>
+      <c r="D46" s="11">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E46" s="11">
+        <v>158</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="11">
+        <v>3.452</v>
+      </c>
+      <c r="D47" s="11">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="E47" s="16">
+        <v>318</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="11">
+        <v>3.2370000000000001</v>
+      </c>
+      <c r="D48" s="11">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="E48" s="11">
+        <v>60</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="11">
+        <v>4.22</v>
+      </c>
+      <c r="D49" s="11">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="E49" s="11">
+        <v>56</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="11">
+        <v>3.9649999999999999</v>
+      </c>
+      <c r="D50" s="11">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E50" s="11">
+        <v>38</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="11">
+        <v>3.6280000000000001</v>
+      </c>
+      <c r="D51" s="11">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="E51" s="11">
+        <v>72</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" s="11">
+        <v>4.1609999999999996</v>
+      </c>
+      <c r="D52" s="11">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E52" s="11">
+        <v>10</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="11">
+        <v>2.9</v>
+      </c>
+      <c r="D53" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E53" s="11">
+        <v>40</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="11">
+        <v>3.0950000000000002</v>
+      </c>
+      <c r="D54" s="11">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="E54" s="11">
+        <v>42</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G54" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="11">
+        <v>4.0789999999999997</v>
+      </c>
+      <c r="D55" s="16">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="E55" s="16">
+        <v>24</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="11">
+        <v>5.2830000000000004</v>
+      </c>
+      <c r="D56" s="11">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E56" s="11">
+        <v>6</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="11">
+        <v>3.984</v>
+      </c>
+      <c r="D57" s="11">
+        <v>6.2E-2</v>
+      </c>
+      <c r="E57" s="11">
+        <v>9</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="11">
+        <v>3.6579999999999999</v>
+      </c>
+      <c r="D58" s="11">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="E58" s="11">
+        <v>6</v>
+      </c>
+      <c r="F58" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="11">
+        <v>4.242</v>
+      </c>
+      <c r="D59" s="11">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E59" s="11">
+        <v>3</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="11">
+        <v>5.4</v>
+      </c>
+      <c r="D60" s="11">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E60" s="22">
+        <v>1392</v>
+      </c>
+      <c r="F60" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G60" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="22">
+        <v>3.5</v>
+      </c>
+      <c r="D61" s="22">
+        <v>13.3</v>
+      </c>
+      <c r="E61" s="22">
+        <v>109</v>
+      </c>
+      <c r="F61" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G61" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="22">
+        <v>3.1</v>
+      </c>
+      <c r="D62" s="22">
+        <v>15.2</v>
+      </c>
+      <c r="E62" s="22">
+        <v>131</v>
+      </c>
+      <c r="F62" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G62" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D63" s="22">
+        <v>9.9</v>
+      </c>
+      <c r="E63" s="22">
+        <v>203</v>
+      </c>
+      <c r="F63" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G63" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="11">
+        <v>8.1</v>
+      </c>
+      <c r="D64" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="E64" s="22">
+        <v>318</v>
+      </c>
+      <c r="F64" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="D65" s="11">
+        <v>13.2</v>
+      </c>
+      <c r="E65" s="22">
+        <v>98</v>
+      </c>
+      <c r="F65" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G65" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="11">
+        <v>13.2</v>
+      </c>
+      <c r="D66" s="11">
+        <v>4.3</v>
+      </c>
+      <c r="E66" s="22">
+        <v>264</v>
+      </c>
+      <c r="F66" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G66" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="11">
+        <v>7.7</v>
+      </c>
+      <c r="D67" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="E67" s="22">
+        <v>101</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G67" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="11">
+        <v>5.7</v>
+      </c>
+      <c r="D68" s="11">
+        <v>7.9</v>
+      </c>
+      <c r="E68" s="22">
+        <v>106</v>
+      </c>
+      <c r="F68" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G68" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C69" s="11">
+        <v>6.6</v>
+      </c>
+      <c r="D69" s="11">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E69" s="11">
+        <v>1268</v>
+      </c>
+      <c r="F69" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G69" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="22">
+        <v>3.9</v>
+      </c>
+      <c r="D70" s="22">
+        <v>12.2</v>
+      </c>
+      <c r="E70" s="22">
+        <v>107</v>
+      </c>
+      <c r="F70" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G70" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D71" s="22">
+        <v>12.8</v>
+      </c>
+      <c r="E71" s="22">
+        <v>105</v>
+      </c>
+      <c r="F71" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G71" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="11">
+        <v>6.2</v>
+      </c>
+      <c r="D72" s="22">
+        <v>8.5</v>
+      </c>
+      <c r="E72" s="22">
+        <v>183</v>
+      </c>
+      <c r="F72" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G72" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" s="11">
+        <v>10.3</v>
+      </c>
+      <c r="D73" s="11">
+        <v>5.7</v>
+      </c>
+      <c r="E73" s="11">
+        <v>300</v>
+      </c>
+      <c r="F73" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G73" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="11">
+        <v>3.6</v>
+      </c>
+      <c r="D74" s="11">
+        <v>13.7</v>
+      </c>
+      <c r="E74" s="11">
+        <v>84</v>
+      </c>
+      <c r="F74" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G74" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="11">
+        <v>16.5</v>
+      </c>
+      <c r="D75" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="E75" s="11">
+        <v>252</v>
+      </c>
+      <c r="F75" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="11">
+        <v>11.6</v>
+      </c>
+      <c r="D76" s="11">
+        <v>4.8</v>
+      </c>
+      <c r="E76" s="11">
+        <v>91</v>
+      </c>
+      <c r="F76" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G76" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="D77" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="E77" s="11">
+        <v>96</v>
+      </c>
+      <c r="F77" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G77" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C78" s="11">
+        <v>3.4</v>
+      </c>
+      <c r="D78" s="11">
+        <v>9.4</v>
+      </c>
+      <c r="E78" s="11">
+        <v>116</v>
+      </c>
+      <c r="F78" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G78" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="22">
+        <v>2.6</v>
+      </c>
+      <c r="D79" s="22">
+        <v>11.3</v>
+      </c>
+      <c r="E79" s="22">
+        <v>20</v>
+      </c>
+      <c r="F79" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G79" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="22">
+        <v>3.3</v>
+      </c>
+      <c r="D80" s="22">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E80" s="22">
+        <v>20</v>
+      </c>
+      <c r="F80" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G80" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" s="11">
+        <v>2.9</v>
+      </c>
+      <c r="D81" s="11">
+        <v>12.5</v>
+      </c>
+      <c r="E81" s="11">
+        <v>18</v>
+      </c>
+      <c r="F81" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G81" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="11">
+        <v>6.7</v>
+      </c>
+      <c r="D82" s="11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E82" s="11">
+        <v>14</v>
+      </c>
+      <c r="F82" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G82" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" s="11">
+        <v>5.8</v>
+      </c>
+      <c r="D83" s="11">
+        <v>5.8</v>
+      </c>
+      <c r="E83" s="11">
+        <v>12</v>
+      </c>
+      <c r="F83" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G83" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D84" s="11">
+        <v>18.2</v>
+      </c>
+      <c r="E84" s="11">
+        <v>10</v>
+      </c>
+      <c r="F84" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G84" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B85" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" s="11">
+        <v>7.8</v>
+      </c>
+      <c r="D85" s="11">
+        <v>3.4</v>
+      </c>
+      <c r="E85" s="11">
+        <v>10</v>
+      </c>
+      <c r="F85" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G85" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B86" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86" s="11">
+        <v>7.1980000000000004</v>
+      </c>
+      <c r="D86" s="11">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="E86" s="22">
+        <v>1392</v>
+      </c>
+      <c r="F86" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G86" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D87" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="E87" s="22">
+        <v>109</v>
+      </c>
+      <c r="F87" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G87" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B88" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="11">
+        <v>3.89</v>
+      </c>
+      <c r="D88" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="E88" s="22">
+        <v>131</v>
+      </c>
+      <c r="F88" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G88" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="11">
+        <v>7.1909999999999998</v>
+      </c>
+      <c r="D89" s="11">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="E89" s="22">
+        <v>203</v>
+      </c>
+      <c r="F89" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G89" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B90" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="11">
+        <v>11.74</v>
+      </c>
+      <c r="D90" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="E90" s="22">
+        <v>318</v>
+      </c>
+      <c r="F90" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G90" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="11">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D91" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E91" s="22">
+        <v>98</v>
+      </c>
+      <c r="F91" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G91" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="11">
+        <v>18.898</v>
+      </c>
+      <c r="D92" s="11">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E92" s="22">
+        <v>264</v>
+      </c>
+      <c r="F92" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G92" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="11">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="D93" s="11">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="E93" s="22">
+        <v>101</v>
+      </c>
+      <c r="F93" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G93" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B94" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C94" s="11">
+        <v>6.0570000000000004</v>
+      </c>
+      <c r="D94" s="11">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="E94" s="22">
+        <v>106</v>
+      </c>
+      <c r="F94" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="G94" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B95" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="11">
+        <v>9.7810000000000006</v>
+      </c>
+      <c r="D95" s="11">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="E95" s="11">
+        <v>1268</v>
+      </c>
+      <c r="F95" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G95" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B96" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96" s="11">
+        <v>5.7530000000000001</v>
+      </c>
+      <c r="D96" s="11">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="E96" s="11">
+        <v>107</v>
+      </c>
+      <c r="F96" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G96" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B97" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97" s="11">
+        <v>5.798</v>
+      </c>
+      <c r="D97" s="11">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="E97" s="11">
+        <v>105</v>
+      </c>
+      <c r="F97" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G97" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B98" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="11">
+        <v>9.7170000000000005</v>
+      </c>
+      <c r="D98" s="11">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="E98" s="11">
+        <v>183</v>
+      </c>
+      <c r="F98" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G98" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" s="11">
+        <v>16.962</v>
+      </c>
+      <c r="D99" s="11">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E99" s="11">
+        <v>300</v>
+      </c>
+      <c r="F99" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G99" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" s="11">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="D100" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E100" s="11">
+        <v>84</v>
+      </c>
+      <c r="F100" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G100" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B101" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" s="11">
+        <v>28.835999999999999</v>
+      </c>
+      <c r="D101" s="11">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E101" s="11">
+        <v>252</v>
+      </c>
+      <c r="F101" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G101" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B102" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="11">
+        <v>18.706</v>
+      </c>
+      <c r="D102" s="11">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E102" s="11">
+        <v>91</v>
+      </c>
+      <c r="F102" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G102" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103" s="11">
+        <v>7.1449999999999996</v>
+      </c>
+      <c r="D103" s="11">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="E103" s="11">
+        <v>96</v>
+      </c>
+      <c r="F103" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G103" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B104" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="11">
+        <v>3.8119999999999998</v>
+      </c>
+      <c r="D104" s="11">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="E104" s="11">
+        <v>116</v>
+      </c>
+      <c r="F104" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G104" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B105" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C105" s="11">
+        <v>3.02</v>
+      </c>
+      <c r="D105" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E105" s="11">
+        <v>20</v>
+      </c>
+      <c r="F105" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G105" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B106" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" s="11">
+        <v>4.18</v>
+      </c>
+      <c r="D106" s="11">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E106" s="11">
+        <v>20</v>
+      </c>
+      <c r="F106" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G106" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B107" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107" s="11">
+        <v>3.4</v>
+      </c>
+      <c r="D107" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E107" s="11">
+        <v>18</v>
+      </c>
+      <c r="F107" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G107" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B108" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C108" s="11">
+        <v>10.005000000000001</v>
+      </c>
+      <c r="D108" s="11">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E108" s="11">
+        <v>14</v>
+      </c>
+      <c r="F108" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G108" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B109" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" s="11">
+        <v>6.9359999999999999</v>
+      </c>
+      <c r="D109" s="11">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E109" s="11">
+        <v>12</v>
+      </c>
+      <c r="F109" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G109" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B110" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110" s="11">
+        <v>1.96</v>
+      </c>
+      <c r="D110" s="11">
+        <v>0.24</v>
+      </c>
+      <c r="E110" s="11">
+        <v>10</v>
+      </c>
+      <c r="F110" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G110" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B111" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C111" s="11">
+        <v>6.0039999999999996</v>
+      </c>
+      <c r="D111" s="11">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E111" s="11">
+        <v>10</v>
+      </c>
+      <c r="F111" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G111" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G53" sqref="A1:G53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="11">
+        <v>5.4</v>
+      </c>
+      <c r="D2" s="11">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1392</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="D3" s="9">
+        <v>13.3</v>
+      </c>
+      <c r="E3" s="9">
+        <v>109</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3.1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>15.2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>131</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D5" s="9">
+        <v>9.9</v>
+      </c>
+      <c r="E5" s="9">
+        <v>203</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="18">
+        <v>8.1</v>
+      </c>
+      <c r="D6" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>318</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="D7" s="11">
+        <v>13.2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>98</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="18">
+        <v>13.2</v>
+      </c>
+      <c r="D8" s="11">
+        <v>4.3</v>
+      </c>
+      <c r="E8" s="9">
+        <v>264</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="18">
+        <v>7.7</v>
+      </c>
+      <c r="D9" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>101</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="11">
+        <v>5.7</v>
+      </c>
+      <c r="D10" s="11">
+        <v>7.9</v>
+      </c>
+      <c r="E10" s="9">
+        <v>106</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="11">
+        <v>6.6</v>
+      </c>
+      <c r="D11" s="11">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1268</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <v>3.9</v>
+      </c>
+      <c r="D12" s="9">
+        <v>12.2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>107</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="11">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D13" s="9">
+        <v>12.8</v>
+      </c>
+      <c r="E13" s="9">
+        <v>105</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="11">
+        <v>6.2</v>
+      </c>
+      <c r="D14" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="E14" s="9">
+        <v>183</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="18">
+        <v>10.3</v>
+      </c>
+      <c r="D15" s="11">
+        <v>5.7</v>
+      </c>
+      <c r="E15" s="11">
+        <v>300</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="11">
+        <v>3.6</v>
+      </c>
+      <c r="D16" s="11">
+        <v>13.7</v>
+      </c>
+      <c r="E16" s="11">
+        <v>84</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="18">
+        <v>16.5</v>
+      </c>
+      <c r="D17" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="E17" s="11">
+        <v>252</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18">
+        <v>11.6</v>
+      </c>
+      <c r="D18" s="11">
+        <v>4.8</v>
+      </c>
+      <c r="E18" s="11">
+        <v>91</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="D19" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="E19" s="11">
+        <v>96</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="11">
+        <v>3.4</v>
+      </c>
+      <c r="D20" s="11">
+        <v>9.4</v>
+      </c>
+      <c r="E20" s="11">
+        <v>116</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="9">
+        <v>2.6</v>
+      </c>
+      <c r="D21" s="9">
+        <v>11.3</v>
+      </c>
+      <c r="E21" s="9">
+        <v>20</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="D22" s="9">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E22" s="9">
+        <v>20</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="11">
+        <v>2.9</v>
+      </c>
+      <c r="D23" s="11">
+        <v>12.5</v>
+      </c>
+      <c r="E23" s="11">
+        <v>18</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="11">
+        <v>6.7</v>
+      </c>
+      <c r="D24" s="11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E24" s="11">
+        <v>14</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="11">
+        <v>5.8</v>
+      </c>
+      <c r="D25" s="11">
+        <v>5.8</v>
+      </c>
+      <c r="E25" s="11">
+        <v>12</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D26" s="11">
+        <v>18.2</v>
+      </c>
+      <c r="E26" s="11">
+        <v>10</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="11">
+        <v>7.8</v>
+      </c>
+      <c r="D27" s="11">
+        <v>3.4</v>
+      </c>
+      <c r="E27" s="11">
+        <v>10</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="11">
+        <v>7.1980000000000004</v>
+      </c>
+      <c r="D28" s="11">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1392</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="E29" s="9">
+        <v>109</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="11">
+        <v>3.89</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="E30" s="9">
+        <v>131</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="11">
+        <v>7.1909999999999998</v>
+      </c>
+      <c r="D31" s="11">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="E31" s="9">
+        <v>203</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="18">
+        <v>11.74</v>
+      </c>
+      <c r="D32" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="E32" s="9">
+        <v>318</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="11">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="D33" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E33" s="9">
+        <v>98</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="18">
+        <v>18.898</v>
+      </c>
+      <c r="D34" s="11">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E34" s="9">
+        <v>264</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="18">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="D35" s="11">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="E35" s="9">
+        <v>101</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="11">
+        <v>6.0570000000000004</v>
+      </c>
+      <c r="D36" s="11">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="E36" s="9">
+        <v>106</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="11">
+        <v>9.7810000000000006</v>
+      </c>
+      <c r="D37" s="11">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="E37" s="11">
+        <v>1268</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="11">
+        <v>5.7530000000000001</v>
+      </c>
+      <c r="D38" s="11">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="E38" s="11">
+        <v>107</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="11">
+        <v>5.798</v>
+      </c>
+      <c r="D39" s="11">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="E39" s="11">
+        <v>105</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="11">
+        <v>9.7170000000000005</v>
+      </c>
+      <c r="D40" s="11">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="E40" s="11">
+        <v>183</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="18">
+        <v>16.962</v>
+      </c>
+      <c r="D41" s="11">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E41" s="11">
+        <v>300</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="11">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="D42" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E42" s="11">
+        <v>84</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="18">
+        <v>28.835999999999999</v>
+      </c>
+      <c r="D43" s="11">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E43" s="11">
+        <v>252</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="18">
+        <v>18.706</v>
+      </c>
+      <c r="D44" s="11">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E44" s="11">
+        <v>91</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="11">
+        <v>7.1449999999999996</v>
+      </c>
+      <c r="D45" s="11">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="E45" s="11">
+        <v>96</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="11">
+        <v>3.8119999999999998</v>
+      </c>
+      <c r="D46" s="11">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="E46" s="11">
+        <v>116</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="11">
+        <v>3.02</v>
+      </c>
+      <c r="D47" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E47" s="11">
+        <v>20</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="11">
+        <v>4.18</v>
+      </c>
+      <c r="D48" s="11">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E48" s="11">
+        <v>20</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="11">
+        <v>3.4</v>
+      </c>
+      <c r="D49" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E49" s="11">
+        <v>18</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="18">
+        <v>10.005000000000001</v>
+      </c>
+      <c r="D50" s="11">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E50" s="11">
+        <v>14</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="11">
+        <v>6.9359999999999999</v>
+      </c>
+      <c r="D51" s="11">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E51" s="11">
+        <v>12</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="18">
+        <v>1.96</v>
+      </c>
+      <c r="D52" s="11">
+        <v>0.24</v>
+      </c>
+      <c r="E52" s="11">
+        <v>10</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="11">
+        <v>6.0039999999999996</v>
+      </c>
+      <c r="D53" s="11">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E53" s="11">
+        <v>10</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
small updates to files
</commit_message>
<xml_diff>
--- a/results/gamma_estimates.xlsx
+++ b/results/gamma_estimates.xlsx
@@ -2224,10 +2224,13 @@
   <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">

</xml_diff>